<commit_message>
deleting time from HTML
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1283,6 +1283,240 @@
         <v>5.84</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>شادن</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ق</t>
+        </is>
+      </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>شادن</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ا</t>
+        </is>
+      </c>
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>شادن</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ف</t>
+        </is>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>شادن</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ز</t>
+        </is>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>شادن</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ف</t>
+        </is>
+      </c>
+      <c r="C52" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" t="n">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>شادن</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>ف</t>
+        </is>
+      </c>
+      <c r="C53" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>شادن</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>د</t>
+        </is>
+      </c>
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>شادن</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ف</t>
+        </is>
+      </c>
+      <c r="C55" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>شادن</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>ا</t>
+        </is>
+      </c>
+      <c r="C56" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>شادن</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>د</t>
+        </is>
+      </c>
+      <c r="C57" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ٍshaden</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>س</t>
+        </is>
+      </c>
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>shaden</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>س</t>
+        </is>
+      </c>
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>shaden</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ه</t>
+        </is>
+      </c>
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix some problems xD
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1877,6 +1877,168 @@
         <v>0</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>د</t>
+        </is>
+      </c>
+      <c r="C81" t="b">
+        <v>0</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Abdulkarim Almalki</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>م</t>
+        </is>
+      </c>
+      <c r="C82" t="b">
+        <v>0</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Abdulkarim Almalki</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>ا</t>
+        </is>
+      </c>
+      <c r="C83" t="b">
+        <v>0</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>qqqqqqq</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>م</t>
+        </is>
+      </c>
+      <c r="C84" t="b">
+        <v>1</v>
+      </c>
+      <c r="D84" t="n">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>ت</t>
+        </is>
+      </c>
+      <c r="C85" t="b">
+        <v>1</v>
+      </c>
+      <c r="D85" t="n">
+        <v>4.06</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>aaaaaa</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>ل</t>
+        </is>
+      </c>
+      <c r="C86" t="b">
+        <v>0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>aaaaaa</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>ج</t>
+        </is>
+      </c>
+      <c r="C87" t="b">
+        <v>1</v>
+      </c>
+      <c r="D87" t="n">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>aaaaaa</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>ز</t>
+        </is>
+      </c>
+      <c r="C88" t="b">
+        <v>0</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>EEE</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>ن</t>
+        </is>
+      </c>
+      <c r="C89" t="b">
+        <v>0</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>